<commit_message>
Más sobre manejo de Celdas
</commit_message>
<xml_diff>
--- a/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
+++ b/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="11440" yWindow="460" windowWidth="17360" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="EntradasSalidas">Hoja1!$A$4:$C$7</definedName>
+    <definedName name="EntradasSalidas">Hoja1!$A$5:$C$8</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +32,7 @@
     <author>Usuario de Microsoft Office</author>
   </authors>
   <commentList>
-    <comment ref="B8" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,51 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="H9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma con su respectiva función</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma a partir de formulas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t xml:space="preserve">MES </t>
   </si>
@@ -164,6 +208,15 @@
       <t>datoF:datoK).</t>
     </r>
   </si>
+  <si>
+    <t>Sucursal 1 - Entradas Salidas</t>
+  </si>
+  <si>
+    <t>Sucursal 2 - Entradas Salidas</t>
+  </si>
+  <si>
+    <t>Abr</t>
+  </si>
 </sst>
 </file>
 
@@ -172,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,6 +288,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -274,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -396,13 +456,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -434,6 +531,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -714,190 +823,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="F3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="F5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>150</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="15">
-        <f>B5-C5</f>
+      <c r="D6" s="15">
+        <f>B6-C6</f>
         <v>50</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>150</v>
+      </c>
+      <c r="H6" s="3">
+        <v>100</v>
+      </c>
+      <c r="I6" s="15">
+        <f>G6-H6</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="5">
         <v>330</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="6">
         <v>250</v>
       </c>
-      <c r="D6" s="15">
-        <f t="shared" ref="D6:D7" si="0">B6-C6</f>
+      <c r="D7" s="15">
+        <f t="shared" ref="D7:D9" si="0">B7-C7</f>
         <v>80</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>330</v>
+      </c>
+      <c r="H7" s="6">
+        <v>250</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" ref="I7:I8" si="1">G7-H7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B8" s="8">
         <v>225</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C8" s="9">
         <v>180</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D8" s="15">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="F8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="8">
+        <v>225</v>
+      </c>
+      <c r="H8" s="9">
+        <v>180</v>
+      </c>
+      <c r="I8" s="15">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <v>425</v>
+      </c>
+      <c r="C9" s="6">
+        <v>285</v>
+      </c>
+      <c r="D9" s="15">
+        <f>B9-C9</f>
+        <v>140</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15">
-        <f>B5+B6+B7</f>
+      <c r="G9" s="15">
+        <f>G6+G7+G8</f>
         <v>705</v>
       </c>
-      <c r="C8" s="15">
-        <f>SUM(C5:C7)</f>
+      <c r="H9" s="15">
+        <f>SUM(H6:H8)</f>
         <v>530</v>
       </c>
-      <c r="D8" s="17">
-        <f t="shared" ref="D8" si="1">SUM(D5:D7)</f>
+      <c r="I9" s="17">
+        <f t="shared" ref="I9" si="2">SUM(I6:I8)</f>
         <v>175</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F11" s="19" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="15">
+        <f>SUM(B6:B9)</f>
+        <v>1130</v>
+      </c>
+      <c r="C10" s="15">
+        <f>SUM(C6:C9)</f>
+        <v>815</v>
+      </c>
+      <c r="D10" s="17">
+        <f>SUM(D6:D9)</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F19" s="19" t="s">
         <v>10</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="19" spans="6:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F19" s="19" t="s">
-        <v>11</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -918,11 +1092,65 @@
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
     </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F27" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F4:J9"/>
-    <mergeCell ref="F11:J17"/>
-    <mergeCell ref="F19:J22"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F12:J17"/>
+    <mergeCell ref="F19:J25"/>
+    <mergeCell ref="F27:J30"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Avances en visualizaciones, analisis de datos
</commit_message>
<xml_diff>
--- a/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
+++ b/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
@@ -5,17 +5,19 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertovelasquezdean/Desktop/Rescata_/Programación/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertovelasquezdean/Desktop/Rescata_/Programación/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="460" windowWidth="17360" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sucursal_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sucursal_2" sheetId="2" r:id="rId2"/>
+    <sheet name="Totales" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="EntradasSalidas">Hoja1!$A$5:$C$8</definedName>
+    <definedName name="EntradasSalidas">Sucursal_1!$A$5:$C$8</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,50 +34,6 @@
     <author>Usuario de Microsoft Office</author>
   </authors>
   <commentList>
-    <comment ref="G9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Usuario de Microsoft Office:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Operación Suma a partir de formulas</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Usuario de Microsoft Office:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Operación Suma con su respectiva función</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B10" authorId="0">
       <text>
         <r>
@@ -124,8 +82,139 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario de Microsoft Office</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma a partir de formulas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma con su respectiva función</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario de Microsoft Office</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Tipo de reporte o práctica que consiste en importar datos de otra hoja de cálculo de un mismo archivo Excel.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma a partir de formulas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Operación Suma con su respectiva función</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t xml:space="preserve">MES </t>
   </si>
@@ -217,6 +306,24 @@
   <si>
     <t>Abr</t>
   </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>SUCURSAL</t>
+  </si>
+  <si>
+    <t>Sucursal 1</t>
+  </si>
+  <si>
+    <t>Sucursal 2</t>
+  </si>
+  <si>
+    <t>Práctica: Consolidado de datos manualmente</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +332,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,8 +402,30 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +460,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -499,7 +634,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -524,17 +659,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,6 +669,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -823,43 +965,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="F3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -874,18 +1010,13 @@
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>7</v>
-      </c>
+      <c r="F5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -901,19 +1032,11 @@
         <f>B6-C6</f>
         <v>50</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>150</v>
-      </c>
-      <c r="H6" s="3">
-        <v>100</v>
-      </c>
-      <c r="I6" s="15">
-        <f>G6-H6</f>
-        <v>50</v>
-      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -926,22 +1049,14 @@
         <v>250</v>
       </c>
       <c r="D7" s="15">
-        <f t="shared" ref="D7:D9" si="0">B7-C7</f>
+        <f t="shared" ref="D7:D8" si="0">B7-C7</f>
         <v>80</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="5">
-        <v>330</v>
-      </c>
-      <c r="H7" s="6">
-        <v>250</v>
-      </c>
-      <c r="I7" s="15">
-        <f t="shared" ref="I7:I8" si="1">G7-H7</f>
-        <v>80</v>
-      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -957,19 +1072,11 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="8">
-        <v>225</v>
-      </c>
-      <c r="H8" s="9">
-        <v>180</v>
-      </c>
-      <c r="I8" s="15">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -985,24 +1092,14 @@
         <f>B9-C9</f>
         <v>140</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="15">
-        <f>G6+G7+G8</f>
-        <v>705</v>
-      </c>
-      <c r="H9" s="15">
-        <f>SUM(H6:H8)</f>
-        <v>530</v>
-      </c>
-      <c r="I9" s="17">
-        <f t="shared" ref="I9" si="2">SUM(I6:I8)</f>
-        <v>175</v>
-      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="15">
@@ -1013,147 +1110,345 @@
         <f>SUM(C6:C9)</f>
         <v>815</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <f>SUM(D6:D9)</f>
         <v>315</v>
       </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="F12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F19" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="20" spans="6:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="F20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F27" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F12:J17"/>
-    <mergeCell ref="F19:J25"/>
-    <mergeCell ref="F27:J30"/>
+    <mergeCell ref="F5:J10"/>
+    <mergeCell ref="F12:J18"/>
+    <mergeCell ref="F20:J23"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>150</v>
+      </c>
+      <c r="C6" s="3">
+        <v>100</v>
+      </c>
+      <c r="D6" s="15">
+        <f>B6-C6</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>330</v>
+      </c>
+      <c r="C7" s="6">
+        <v>250</v>
+      </c>
+      <c r="D7" s="15">
+        <f>B7-C7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>225</v>
+      </c>
+      <c r="C8" s="9">
+        <v>180</v>
+      </c>
+      <c r="D8" s="15">
+        <f>B8-C8</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <f>B6+B7+B8</f>
+        <v>705</v>
+      </c>
+      <c r="C9" s="15">
+        <f>SUM(C6:C8)</f>
+        <v>530</v>
+      </c>
+      <c r="D9" s="16">
+        <f>SUM(D6:D8)</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <f>Sucursal_1!B10</f>
+        <v>1130</v>
+      </c>
+      <c r="C6" s="1">
+        <f>Sucursal_1!C10</f>
+        <v>815</v>
+      </c>
+      <c r="D6" s="15">
+        <f>Sucursal_1!D10</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
+        <f>Sucursal_2!B9</f>
+        <v>705</v>
+      </c>
+      <c r="C7" s="5">
+        <f>Sucursal_2!C9</f>
+        <v>530</v>
+      </c>
+      <c r="D7" s="15">
+        <f>Sucursal_2!D9</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="15">
+        <f>B8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27">
+        <f>B6+B7+B8</f>
+        <v>1835</v>
+      </c>
+      <c r="C9" s="27">
+        <f>SUM(C6:C8)</f>
+        <v>1345</v>
+      </c>
+      <c r="D9" s="28">
+        <f>SUM(D6:D8)</f>
+        <v>490</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atajos y Referencias Absolutas
</commit_message>
<xml_diff>
--- a/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
+++ b/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/Entradas & Salidas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertovelasquezdean/Desktop/Rescata_/Programación/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertovelasquezdean/Desktop/Rescata_/Programación/Excel/Práctica/2. Manejo de Celdas, Fórmulas y Funciones en Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,6 +165,229 @@
         </r>
       </text>
     </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Usuario de Microsoft Office:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+En pocas palabras, se habla de</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>referencia absoluta</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> cuando queremos fijar, operativamente hablando, una celda en especifica según se corra una formula o función, a partir de la misma; de manera horizontal, vertical o en ambos sentidos (referencia absoluta total). Es decir, si determinamos que al correr una formula o función, a partir de una celda, esta celda se mantenga completamente involucrada (fija) dentro de las operaciones siguientes; le estamos dando a dicha celda una referencia absoluta. 
+Ahora, la referencia absoluta puede ser parcial (vertical u horizontal) o total. Una celda con referencia absoluta en su sentido vertical (con el simbolo </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>$</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> en la parte númerica de una celda; por ejemplo: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>A$1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">); quiere decir que, al correr una formula o función entre las demás celdas, </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>verticalmente,</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> y desde ella misma, ésta se mantendrá involucrada y </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>fija</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> en las sub-siguientes operaciones matematicas con las posteriores celdas en juego.
+Una celda con referencia absoluta, pero ahora en su sentido horizontal (con el simbolo </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>$</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> en la parte alfabetica de una celda; por ejemplo: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>$A1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">); quiere decir que, al correr una formula o función entre las demás celdas, </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>horizontalmente,</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> y desde ella misma, ésta se mantendrá involucrada y </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>fija</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> en las sub-siguientes operaciones matematicas con las posteriores celdas en juego. Pruebelo usted mismo con los </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>totales</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>de su resumen.
+Puede imaginar entonces qué acontencería si ve esto "</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>$A$1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>" al correr celdas desde ella.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B9" authorId="0">
       <text>
         <r>
@@ -214,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t xml:space="preserve">MES </t>
   </si>
@@ -324,6 +547,55 @@
   <si>
     <t>Práctica: Consolidado de datos manualmente</t>
   </si>
+  <si>
+    <t>Práctica: Referencias absolutas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Command + 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sobre una celda y cambia su formato</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Command + 0 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sobre columna para ocultarla</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -332,7 +604,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -421,6 +693,33 @@
       <b/>
       <sz val="12"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -634,7 +933,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -685,6 +984,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1345,7 +1650,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1368,6 +1673,12 @@
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
+      <c r="F3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1382,6 +1693,12 @@
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
+      <c r="F5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
@@ -1408,7 +1725,7 @@
         <f>Sucursal_2!B9</f>
         <v>705</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="30">
         <f>Sucursal_2!C9</f>
         <v>530</v>
       </c>
@@ -1416,6 +1733,12 @@
         <f>Sucursal_2!D9</f>
         <v>175</v>
       </c>
+      <c r="F7" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
@@ -1444,11 +1767,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>